<commit_message>
Tuning parameters and analyzing
</commit_message>
<xml_diff>
--- a/ATC/Forecast/Pop/population_production_h8.xlsx
+++ b/ATC/Forecast/Pop/population_production_h8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/lholguin_purdue_edu/Documents/VS code/Data/ATC/Forecast/Pop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_EB5F2F57C8F74085550E51C017EE8A1440B404F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42C3B378-C59C-4DF6-8C75-BD09CD66BBD6}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_EB5F2F57C8F74085550E51C017EE8A1440B404F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B2D039-7D0D-4384-9618-B279DFF2BEA5}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2860" yWindow="2990" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_Models" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -238,7 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,6 +254,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2706,7 +2710,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:G33"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2921,7 +2925,7 @@
         <v>3582938.1347745941</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>1896367.497943769</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2967,7 +2971,7 @@
         <v>1962949.8742151749</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2990,7 +2994,7 @@
         <v>2032674.402617584</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3013,7 +3017,7 @@
         <v>2101375.80944773</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3036,7 +3040,7 @@
         <v>2167281.4148276029</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3059,7 +3063,7 @@
         <v>2229717.893320879</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3082,7 +3086,7 @@
         <v>2288545.8916620719</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3289,7 +3293,7 @@
         <v>3252929.7968900031</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3312,7 +3316,7 @@
         <v>3190123.591178461</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3335,7 +3339,7 @@
         <v>3276720.7081793938</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3358,7 +3362,7 @@
         <v>3366143.9435306829</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -3381,7 +3385,7 @@
         <v>3454669.9996846439</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -3404,7 +3408,7 @@
         <v>3540344.7866240898</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -3427,7 +3431,7 @@
         <v>3622277.0017208531</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3450,7 +3454,7 @@
         <v>3700162.9354691049</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -3477,7 +3481,7 @@
   <autoFilter ref="A1:G33" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="OH"/>
+        <filter val="IN"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>